<commit_message>
Progress on calculation of Total_Calories
</commit_message>
<xml_diff>
--- a/data/Calorias por edad.xlsx
+++ b/data/Calorias por edad.xlsx
@@ -1,30 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\3. Propuestas\Distance Education\SEA004\Mapas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kei\Documents\GitHub\FS-Security\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF00403E-EFAB-4AA0-81D8-79737185A7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12315"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Edad</t>
   </si>
@@ -33,12 +45,51 @@
   </si>
   <si>
     <t>Caloriasmujer</t>
+  </si>
+  <si>
+    <t>Agrupacion de Edades 0-4</t>
+  </si>
+  <si>
+    <t>Agrupacion de Edades 5-9</t>
+  </si>
+  <si>
+    <t>Agrupacion de Edades 10-14</t>
+  </si>
+  <si>
+    <t>Agrupacion de Edades 15-19</t>
+  </si>
+  <si>
+    <t>Agrupacion de Edades 20-24</t>
+  </si>
+  <si>
+    <t>Agrupacion de Edades 25-34</t>
+  </si>
+  <si>
+    <t>Agrupacion de Edades 35-44</t>
+  </si>
+  <si>
+    <t>Agrupacion de Edades 45-54</t>
+  </si>
+  <si>
+    <t>Agrupacion de Edades 55-59</t>
+  </si>
+  <si>
+    <t>Agrupacion de Edades 60-64</t>
+  </si>
+  <si>
+    <t>Agrupacion de Edades 65-74</t>
+  </si>
+  <si>
+    <t>Agrupacion de Edades 75-84</t>
+  </si>
+  <si>
+    <t>Agrupacion de Edades 85+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -349,16 +400,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C87"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -368,8 +419,47 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -379,8 +469,12 @@
       <c r="C2">
         <v>1000</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>SUM(B2:B6)</f>
+        <v>5920.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -391,7 +485,7 @@
         <v>1047.3599999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -402,7 +496,7 @@
         <v>1094.72</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -413,7 +507,7 @@
         <v>1142.08</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -424,7 +518,7 @@
         <v>1189.44</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -435,7 +529,7 @@
         <v>1236.8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -446,7 +540,7 @@
         <v>1284.1599999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -457,7 +551,7 @@
         <v>1331.52</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -468,7 +562,7 @@
         <v>1378.88</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -479,7 +573,7 @@
         <v>1426.24</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -490,7 +584,7 @@
         <v>1473.6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -501,7 +595,7 @@
         <v>1520.96</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -512,7 +606,7 @@
         <v>1568.32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -523,7 +617,7 @@
         <v>1615.6799999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -534,7 +628,7 @@
         <v>1663.04</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -545,7 +639,7 @@
         <v>1710.4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -556,7 +650,7 @@
         <v>1757.76</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -567,7 +661,7 @@
         <v>1805.12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -578,7 +672,7 @@
         <v>1852.48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -589,7 +683,7 @@
         <v>1843.19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -600,7 +694,7 @@
         <v>1838.3000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -611,7 +705,7 @@
         <v>1833.4099999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -622,7 +716,7 @@
         <v>1828.52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -633,7 +727,7 @@
         <v>1823.6299999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -644,7 +738,7 @@
         <v>1818.7399999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -655,7 +749,7 @@
         <v>1813.85</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -666,7 +760,7 @@
         <v>1808.9599999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -677,7 +771,7 @@
         <v>1804.0700000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -688,7 +782,7 @@
         <v>1799.1799999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -699,7 +793,7 @@
         <v>1794.29</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -710,7 +804,7 @@
         <v>1789.4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -721,7 +815,7 @@
         <v>1784.5099999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -732,7 +826,7 @@
         <v>1779.62</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -743,7 +837,7 @@
         <v>1774.73</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -754,7 +848,7 @@
         <v>1769.8399999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -765,7 +859,7 @@
         <v>1764.9499999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -776,7 +870,7 @@
         <v>1760.06</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -787,7 +881,7 @@
         <v>1755.1699999999996</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -798,7 +892,7 @@
         <v>1750.2800000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -809,7 +903,7 @@
         <v>1745.3899999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -820,7 +914,7 @@
         <v>1740.5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -831,7 +925,7 @@
         <v>1735.6100000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -842,7 +936,7 @@
         <v>1730.7199999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -853,7 +947,7 @@
         <v>1725.83</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -864,7 +958,7 @@
         <v>1720.94</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -875,7 +969,7 @@
         <v>1716.0499999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -886,7 +980,7 @@
         <v>1711.1599999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -897,7 +991,7 @@
         <v>1706.2700000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -908,7 +1002,7 @@
         <v>1701.38</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -919,7 +1013,7 @@
         <v>1696.4899999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -930,7 +1024,7 @@
         <v>1691.6000000000004</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -941,7 +1035,7 @@
         <v>1686.71</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -952,7 +1046,7 @@
         <v>1681.8199999999997</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -963,7 +1057,7 @@
         <v>1676.9300000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -974,7 +1068,7 @@
         <v>1672.04</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -985,7 +1079,7 @@
         <v>1667.1500000000005</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -996,7 +1090,7 @@
         <v>1662.2600000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1007,7 +1101,7 @@
         <v>1657.37</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1018,7 +1112,7 @@
         <v>1652.4800000000005</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -1029,7 +1123,7 @@
         <v>1647.5900000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -1040,7 +1134,7 @@
         <v>1642.6999999999998</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -1051,7 +1145,7 @@
         <v>1637.8100000000004</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -1062,7 +1156,7 @@
         <v>1632.92</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -1073,7 +1167,7 @@
         <v>1628.0299999999997</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -1084,7 +1178,7 @@
         <v>1623.1400000000003</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -1095,7 +1189,7 @@
         <v>1618.25</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -1106,7 +1200,7 @@
         <v>1613.3600000000006</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -1117,7 +1211,7 @@
         <v>1608.4700000000003</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -1128,7 +1222,7 @@
         <v>1603.58</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -1139,7 +1233,7 @@
         <v>1598.6900000000005</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -1150,7 +1244,7 @@
         <v>1593.8000000000002</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -1161,7 +1255,7 @@
         <v>1588.9099999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
@@ -1172,7 +1266,7 @@
         <v>1584.0200000000004</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -1183,7 +1277,7 @@
         <v>1579.13</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -1194,7 +1288,7 @@
         <v>1574.2399999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -1205,7 +1299,7 @@
         <v>1569.3500000000004</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -1216,7 +1310,7 @@
         <v>1564.4600000000009</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -1227,7 +1321,7 @@
         <v>1559.5699999999997</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
@@ -1238,7 +1332,7 @@
         <v>1554.6800000000003</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
@@ -1249,7 +1343,7 @@
         <v>1549.7900000000009</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
@@ -1260,7 +1354,7 @@
         <v>1544.9000000000005</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
@@ -1271,7 +1365,7 @@
         <v>1540.0100000000002</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
@@ -1282,7 +1376,7 @@
         <v>1535.1200000000008</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -1293,7 +1387,7 @@
         <v>1530.2300000000005</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
@@ -1304,7 +1398,7 @@
         <v>1525.3400000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>

</xml_diff>